<commit_message>
Ready to put it together
</commit_message>
<xml_diff>
--- a/mergeddata.xlsx
+++ b/mergeddata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Staff Performance Overview" sheetId="1" state="visible" r:id="rId1"/>
@@ -1095,7 +1095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1118,6 +1118,35 @@
       <c r="D2" t="n">
         <v>6</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>4166</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4488.02</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>31.78</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4195.5</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4519.8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1134,6 +1163,35 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>6266.85</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6750.95</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" t="n">
+        <v>21.54</v>
+      </c>
+      <c r="L3" t="n">
+        <v>6286.85</v>
+      </c>
+      <c r="M3" t="n">
+        <v>6772.49</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1149,6 +1207,35 @@
       </c>
       <c r="D4" t="n">
         <v>10</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>596</v>
+      </c>
+      <c r="G4" t="n">
+        <v>641.8</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K4" t="n">
+        <v>32.31</v>
+      </c>
+      <c r="L4" t="n">
+        <v>626</v>
+      </c>
+      <c r="M4" t="n">
+        <v>674.1099999999999</v>
       </c>
     </row>
     <row r="5">

</xml_diff>